<commit_message>
updated template for 0.2.0 for changing defaults
</commit_message>
<xml_diff>
--- a/projects/template_0_2_0_rgenoud.xlsx
+++ b/projects/template_0_2_0_rgenoud.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="10920" windowHeight="9636" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="10920" windowHeight="9636" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="634">
   <si>
     <t>type</t>
   </si>
@@ -1933,6 +1933,9 @@
   </si>
   <si>
     <t>Total Natural Gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change Defaults </t>
   </si>
 </sst>
 </file>
@@ -1999,7 +2002,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2054,6 +2057,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3461,7 +3470,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3542,6 +3551,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5276,8 +5289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5522,7 +5535,9 @@
       <c r="C24" s="12" t="s">
         <v>613</v>
       </c>
-      <c r="D24" s="12"/>
+      <c r="D24" s="40" t="s">
+        <v>633</v>
+      </c>
       <c r="E24" s="14" t="s">
         <v>475</v>
       </c>
@@ -5533,13 +5548,14 @@
         <v>popSize</v>
       </c>
       <c r="B25" s="31">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>30</v>
       </c>
       <c r="C25" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,1,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v>Size of initial population</v>
       </c>
+      <c r="D25" s="41"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="str">
@@ -5547,13 +5563,14 @@
         <v>Generations</v>
       </c>
       <c r="B26" s="31">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>5</v>
       </c>
       <c r="C26" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,2,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v>Number of generations</v>
       </c>
+      <c r="D26" s="41"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="str">
@@ -5561,13 +5578,14 @@
         <v>waitGenerations</v>
       </c>
       <c r="B27" s="31">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D27&lt;&gt;"",D27,IF(LEN(INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>2</v>
       </c>
       <c r="C27" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,3,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v>If no improvement in waitGenerations of generations, then exit</v>
       </c>
+      <c r="D27" s="41"/>
     </row>
     <row r="28" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="str">
@@ -5575,13 +5593,14 @@
         <v>bfgsburnin</v>
       </c>
       <c r="B28" s="31">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D28&lt;&gt;"",D28,IF(LEN(INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>2</v>
       </c>
       <c r="C28" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,4,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v>The number of generations which are run before the BFGS is ﬁrst used</v>
       </c>
+      <c r="D28" s="41"/>
     </row>
     <row r="29" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="37" t="str">
@@ -5589,13 +5608,14 @@
         <v>solutionTolerance</v>
       </c>
       <c r="B29" s="31">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D29&lt;&gt;"",D29,IF(LEN(INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>0.01</v>
       </c>
       <c r="C29" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,5,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v>Numbers within solutionTolerance are considered equal</v>
       </c>
+      <c r="D29" s="41"/>
     </row>
     <row r="30" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="37" t="str">
@@ -5603,13 +5623,14 @@
         <v>epsilonGradient</v>
       </c>
       <c r="B30" s="31">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D30&lt;&gt;"",D30,IF(LEN(INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>0.01</v>
       </c>
       <c r="C30" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,6,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v>epsilon in gradient calculation</v>
       </c>
+      <c r="D30" s="41"/>
     </row>
     <row r="31" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37" t="str">
@@ -5617,13 +5638,14 @@
         <v>pgtol</v>
       </c>
       <c r="B31" s="31">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D31&lt;&gt;"",D31,IF(LEN(INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>0.01</v>
       </c>
       <c r="C31" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,7,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v>tolerance on the projected gradient</v>
       </c>
+      <c r="D31" s="41"/>
     </row>
     <row r="32" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="37" t="str">
@@ -5631,13 +5653,14 @@
         <v>factr</v>
       </c>
       <c r="B32" s="31">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D32&lt;&gt;"",D32,IF(LEN(INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>45036000000000</v>
       </c>
       <c r="C32" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,8,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v>Tolerance on delta_F</v>
       </c>
+      <c r="D32" s="41"/>
     </row>
     <row r="33" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="37" t="str">
@@ -5645,13 +5668,14 @@
         <v>maxit</v>
       </c>
       <c r="B33" s="31">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D33&lt;&gt;"",D33,IF(LEN(INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>100</v>
       </c>
       <c r="C33" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,9,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v>Maximum number of iterations</v>
       </c>
+      <c r="D33" s="41"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="37" t="str">
@@ -5659,13 +5683,14 @@
         <v>normType</v>
       </c>
       <c r="B34" s="31" t="str">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D34&lt;&gt;"",D34,IF(LEN(INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>minkowski</v>
       </c>
       <c r="C34" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$22,10,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v/>
       </c>
+      <c r="D34" s="41"/>
     </row>
     <row r="35" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="37" t="str">
@@ -5673,13 +5698,14 @@
         <v>pPower</v>
       </c>
       <c r="B35" s="31">
-        <f>IF(LEN(INDEX(Lookups!$C$13:$Z$23,11,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$23,11,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))</f>
+        <f>IF(D35&lt;&gt;"",D35,IF(LEN(INDEX(Lookups!$C$13:$Z$23,11,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1))=0,"",INDEX(Lookups!$C$13:$Z$23,11,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)-1)))</f>
         <v>2</v>
       </c>
       <c r="C35" s="32" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$13:$Z$23,11,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))=0,"",INDEX(Lookups!$C$13:$Z$23,11,3*MATCH(Setup!$B21,Lookups!$A$13:$A$19,0)))</f>
         <v>Lp norm power</v>
       </c>
+      <c r="D35" s="41"/>
     </row>
     <row r="36" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="31"/>
@@ -5792,7 +5818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -5848,14 +5874,14 @@
       <c r="R1" s="27"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
-      <c r="U1" s="40" t="s">
+      <c r="U1" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
     </row>
     <row r="2" spans="1:26" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">

</xml_diff>